<commit_message>
Added QuotesPage1 POM Class & Test Class for Same
</commit_message>
<xml_diff>
--- a/src/test/resources/ExcelSheet/PolicyBazaar.xlsx
+++ b/src/test/resources/ExcelSheet/PolicyBazaar.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/06439180ba7c1d53/Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="39" documentId="8_{3C7F3558-0A4B-4542-B64A-592633F2BD90}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4ECDD941-0189-4EEF-84E6-82D61E7C40CE}"/>
+  <xr:revisionPtr revIDLastSave="113" documentId="8_{3C7F3558-0A4B-4542-B64A-592633F2BD90}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0D69FEB1-14E3-4D42-9A96-5E8F6DF166D5}"/>
   <bookViews>
-    <workbookView xWindow="5760" yWindow="3360" windowWidth="17280" windowHeight="8880" xr2:uid="{B5E2913A-31D8-4ED2-9EA3-4C03ADF4D663}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{B5E2913A-31D8-4ED2-9EA3-4C03ADF4D663}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,21 +34,73 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
-  <si>
-    <t>Health Inusrance</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
     <t>View All Products</t>
-  </si>
-  <si>
-    <t>https://health.policybazaar.com/?&amp;utm_content=home_v12_control</t>
   </si>
   <si>
     <t>TEXTS</t>
   </si>
   <si>
     <t>URL</t>
+  </si>
+  <si>
+    <t>LOCATION OF URL</t>
+  </si>
+  <si>
+    <t>https://health.policybazaar.com/v2/proposer/1?utm_content=home_v12_newprequote</t>
+  </si>
+  <si>
+    <t>https://health.policybazaar.com/</t>
+  </si>
+  <si>
+    <t>LANDING PAGE</t>
+  </si>
+  <si>
+    <t>https://health.policybazaar.com/v2/members/2?utm_content=home_v12_newprequote</t>
+  </si>
+  <si>
+    <t>Male</t>
+  </si>
+  <si>
+    <t>Female</t>
+  </si>
+  <si>
+    <t>Your full name</t>
+  </si>
+  <si>
+    <t>QUOTES PAGE1</t>
+  </si>
+  <si>
+    <t>QUOTES PAGE2</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>Full name is required</t>
+  </si>
+  <si>
+    <t>Terms of Use</t>
+  </si>
+  <si>
+    <t>https://www.policybazaar.com/legal-and-admin-policies/</t>
+  </si>
+  <si>
+    <t>https://www.policybazaar.com/legal-and-admin-policies/#termsofuse</t>
+  </si>
+  <si>
+    <t>Health
+Insurance</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Privacy Policy </t>
+  </si>
+  <si>
+    <t>RaJaT</t>
+  </si>
+  <si>
+    <t>Continue ›</t>
   </si>
 </sst>
 </file>
@@ -92,7 +144,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -102,6 +154,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -421,26 +476,29 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1196404-3F35-409E-ACCC-6DF4EAC8152C}">
-  <dimension ref="A1:AB252"/>
+  <dimension ref="A1:AB254"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="22" customWidth="1"/>
     <col min="2" max="2" width="25.5546875" customWidth="1"/>
+    <col min="3" max="3" width="24" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" ht="18" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:28" ht="54" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C1" s="3"/>
       <c r="D1" s="3"/>
       <c r="E1" s="3"/>
       <c r="F1" s="3"/>
@@ -459,14 +517,16 @@
       <c r="S1" s="3"/>
       <c r="T1" s="3"/>
     </row>
-    <row r="2" spans="1:28" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:28" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>0</v>
+        <v>18</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>2</v>
+      <c r="B2" s="4" t="s">
+        <v>5</v>
       </c>
-      <c r="C2" s="1"/>
+      <c r="C2" s="1" t="s">
+        <v>6</v>
+      </c>
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
@@ -493,12 +553,16 @@
       <c r="AA2" s="1"/>
       <c r="AB2" s="1"/>
     </row>
-    <row r="3" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:28" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
-      <c r="B3" s="1"/>
-      <c r="C3" s="1"/>
+      <c r="B3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>11</v>
+      </c>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
@@ -525,10 +589,16 @@
       <c r="AA3" s="1"/>
       <c r="AB3" s="1"/>
     </row>
-    <row r="4" spans="1:28" x14ac:dyDescent="0.3">
-      <c r="A4" s="1"/>
-      <c r="B4" s="1"/>
-      <c r="C4" s="1"/>
+    <row r="4" spans="1:28" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>12</v>
+      </c>
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
@@ -555,10 +625,16 @@
       <c r="AA4" s="1"/>
       <c r="AB4" s="1"/>
     </row>
-    <row r="5" spans="1:28" x14ac:dyDescent="0.3">
-      <c r="A5" s="1"/>
-      <c r="B5" s="1"/>
-      <c r="C5" s="1"/>
+    <row r="5" spans="1:28" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>19</v>
+      </c>
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
@@ -585,10 +661,16 @@
       <c r="AA5" s="1"/>
       <c r="AB5" s="1"/>
     </row>
-    <row r="6" spans="1:28" x14ac:dyDescent="0.3">
-      <c r="A6" s="1"/>
-      <c r="B6" s="1"/>
-      <c r="C6" s="1"/>
+    <row r="6" spans="1:28" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>15</v>
+      </c>
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
@@ -616,7 +698,9 @@
       <c r="AB6" s="1"/>
     </row>
     <row r="7" spans="1:28" x14ac:dyDescent="0.3">
-      <c r="A7" s="1"/>
+      <c r="A7" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
@@ -646,7 +730,9 @@
       <c r="AB7" s="1"/>
     </row>
     <row r="8" spans="1:28" x14ac:dyDescent="0.3">
-      <c r="A8" s="1"/>
+      <c r="A8" s="1" t="s">
+        <v>14</v>
+      </c>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
@@ -676,7 +762,9 @@
       <c r="AB8" s="1"/>
     </row>
     <row r="9" spans="1:28" x14ac:dyDescent="0.3">
-      <c r="A9" s="1"/>
+      <c r="A9" s="1" t="s">
+        <v>21</v>
+      </c>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
@@ -706,7 +794,9 @@
       <c r="AB9" s="1"/>
     </row>
     <row r="10" spans="1:28" x14ac:dyDescent="0.3">
-      <c r="A10" s="1"/>
+      <c r="A10" s="1" t="s">
+        <v>20</v>
+      </c>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
@@ -7995,6 +8085,66 @@
       <c r="AA252" s="1"/>
       <c r="AB252" s="1"/>
     </row>
+    <row r="253" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="A253" s="1"/>
+      <c r="B253" s="1"/>
+      <c r="C253" s="1"/>
+      <c r="D253" s="1"/>
+      <c r="E253" s="1"/>
+      <c r="F253" s="1"/>
+      <c r="G253" s="1"/>
+      <c r="H253" s="1"/>
+      <c r="I253" s="1"/>
+      <c r="J253" s="1"/>
+      <c r="K253" s="1"/>
+      <c r="L253" s="1"/>
+      <c r="M253" s="1"/>
+      <c r="N253" s="1"/>
+      <c r="O253" s="1"/>
+      <c r="P253" s="1"/>
+      <c r="Q253" s="1"/>
+      <c r="R253" s="1"/>
+      <c r="S253" s="1"/>
+      <c r="T253" s="1"/>
+      <c r="U253" s="1"/>
+      <c r="V253" s="1"/>
+      <c r="W253" s="1"/>
+      <c r="X253" s="1"/>
+      <c r="Y253" s="1"/>
+      <c r="Z253" s="1"/>
+      <c r="AA253" s="1"/>
+      <c r="AB253" s="1"/>
+    </row>
+    <row r="254" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="A254" s="1"/>
+      <c r="B254" s="1"/>
+      <c r="C254" s="1"/>
+      <c r="D254" s="1"/>
+      <c r="E254" s="1"/>
+      <c r="F254" s="1"/>
+      <c r="G254" s="1"/>
+      <c r="H254" s="1"/>
+      <c r="I254" s="1"/>
+      <c r="J254" s="1"/>
+      <c r="K254" s="1"/>
+      <c r="L254" s="1"/>
+      <c r="M254" s="1"/>
+      <c r="N254" s="1"/>
+      <c r="O254" s="1"/>
+      <c r="P254" s="1"/>
+      <c r="Q254" s="1"/>
+      <c r="R254" s="1"/>
+      <c r="S254" s="1"/>
+      <c r="T254" s="1"/>
+      <c r="U254" s="1"/>
+      <c r="V254" s="1"/>
+      <c r="W254" s="1"/>
+      <c r="X254" s="1"/>
+      <c r="Y254" s="1"/>
+      <c r="Z254" s="1"/>
+      <c r="AA254" s="1"/>
+      <c r="AB254" s="1"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>